<commit_message>
prepare for google colab
</commit_message>
<xml_diff>
--- a/UvA/LargeDataset/Results.xlsx
+++ b/UvA/LargeDataset/Results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:P1"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,6 +443,60 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>['', '']</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>MetaDiff</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>30</v>
+      </c>
+      <c r="E2" t="n">
+        <v>30</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10</v>
+      </c>
+      <c r="G2" t="n">
+        <v>2</v>
+      </c>
+      <c r="H2" t="n">
+        <v>32</v>
+      </c>
+      <c r="I2" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J2" t="n">
+        <v>256</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.9873920511210893</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.9812361746565094</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.9813206132602249</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.9890020384235453</v>
+      </c>
+      <c r="O2" t="n">
+        <v>404.6989099979401</v>
+      </c>
+      <c r="P2" t="n">
+        <v>202.3413822650909</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Continue with parameters tuning/analysis.
</commit_message>
<xml_diff>
--- a/UvA/LargeDataset/Results.xlsx
+++ b/UvA/LargeDataset/Results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,6 +497,438 @@
         <v>202.3413822650909</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>(0, 0)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>MetaDiff</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>20</v>
+      </c>
+      <c r="F3" t="n">
+        <v>10</v>
+      </c>
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="n">
+        <v>32</v>
+      </c>
+      <c r="I3" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J3" t="n">
+        <v>256</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.9097917965063573</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.9243668538388904</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.9247077910449035</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.9213743551510084</v>
+      </c>
+      <c r="O3" t="n">
+        <v>290.0301671028137</v>
+      </c>
+      <c r="P3" t="n">
+        <v>233.0213561058044</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>(0, 1)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>MetaDiff</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>20</v>
+      </c>
+      <c r="F4" t="n">
+        <v>10</v>
+      </c>
+      <c r="G4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" t="n">
+        <v>32</v>
+      </c>
+      <c r="I4" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J4" t="n">
+        <v>256</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.837295951854823</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.9264414325164468</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.9267729898060869</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.8581380194774533</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.589169979095459</v>
+      </c>
+      <c r="P4" t="n">
+        <v>232.8850328922272</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>(1, 0)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>MetaDiff</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>20</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10</v>
+      </c>
+      <c r="G5" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" t="n">
+        <v>32</v>
+      </c>
+      <c r="I5" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J5" t="n">
+        <v>256</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.9132139471504473</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.9307091467157134</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.9310223889188776</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.9245332691405126</v>
+      </c>
+      <c r="O5" t="n">
+        <v>370.4066350460052</v>
+      </c>
+      <c r="P5" t="n">
+        <v>239.6799750328064</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>(1, 1)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MetaDiff</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>20</v>
+      </c>
+      <c r="F6" t="n">
+        <v>10</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" t="n">
+        <v>32</v>
+      </c>
+      <c r="I6" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J6" t="n">
+        <v>256</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.9140199806766977</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.9302733506434665</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.9305881187538583</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.9251495330680193</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.5930430889129639</v>
+      </c>
+      <c r="P6" t="n">
+        <v>202.437383890152</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>(0, 0)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>MetaDiff</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>10</v>
+      </c>
+      <c r="E7" t="n">
+        <v>20</v>
+      </c>
+      <c r="F7" t="n">
+        <v>10</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" t="n">
+        <v>32</v>
+      </c>
+      <c r="I7" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J7" t="n">
+        <v>256</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.9163044178879687</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.9245029929702727</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.9248428756753467</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.9270024868647453</v>
+      </c>
+      <c r="O7" t="n">
+        <v>280.8699870109558</v>
+      </c>
+      <c r="P7" t="n">
+        <v>216.8287858963013</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>(0, 1)</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>MetaDiff</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" t="n">
+        <v>20</v>
+      </c>
+      <c r="F8" t="n">
+        <v>10</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" t="n">
+        <v>32</v>
+      </c>
+      <c r="I8" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J8" t="n">
+        <v>256</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.9208255071271201</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.9303732654229485</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.9306869878505435</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.9309828542847421</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.5139169692993164</v>
+      </c>
+      <c r="P8" t="n">
+        <v>216.0577948093414</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>(1, 0)</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>MetaDiff</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>10</v>
+      </c>
+      <c r="E9" t="n">
+        <v>20</v>
+      </c>
+      <c r="F9" t="n">
+        <v>10</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" t="n">
+        <v>32</v>
+      </c>
+      <c r="I9" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J9" t="n">
+        <v>256</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.9254896751661508</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.9323896052920266</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.9326939527773629</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.9350107156631599</v>
+      </c>
+      <c r="O9" t="n">
+        <v>297.2036740779877</v>
+      </c>
+      <c r="P9" t="n">
+        <v>221.441232919693</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>(1, 1)</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>MetaDiff</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" t="n">
+        <v>20</v>
+      </c>
+      <c r="F10" t="n">
+        <v>10</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" t="n">
+        <v>32</v>
+      </c>
+      <c r="I10" t="n">
+        <v>50000</v>
+      </c>
+      <c r="J10" t="n">
+        <v>256</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.9282021582337634</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.934215142829811</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.9345115743203479</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.9374128747863907</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.8716640472412109</v>
+      </c>
+      <c r="P10" t="n">
+        <v>246.6976199150085</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>